<commit_message>
added pdf invoice creaton
</commit_message>
<xml_diff>
--- a/app/static/integra_individual_files/2020-10_БДЖ - Пътнически превози_411-2-145_1_integra.xlsx
+++ b/app/static/integra_individual_files/2020-10_БДЖ - Пътнически превози_411-2-145_1_integra.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="53">
   <si>
     <t>№ по ред</t>
   </si>
@@ -97,7 +97,7 @@
     <t>31/10/2020</t>
   </si>
   <si>
-    <t>10/11/2020</t>
+    <t>03/12/2020</t>
   </si>
   <si>
     <t xml:space="preserve"> за м.10.2020г.</t>
@@ -115,6 +115,9 @@
     <t>456-1</t>
   </si>
   <si>
+    <t>11414.853</t>
+  </si>
+  <si>
     <t>100.9000000</t>
   </si>
   <si>
@@ -163,7 +166,7 @@
     <t>411-2-145_1</t>
   </si>
   <si>
-    <t>el.monitoring@agropolychim.bg;m.todorova@agropolychim.bg</t>
+    <t>energy_ee@bdz.bg;vkunova@bdz.bg</t>
   </si>
   <si>
     <t>2020-10_БДЖ - Пътнически превози_411-2-145_1_invoice_reference.xlsx</t>
@@ -629,20 +632,20 @@
       <c r="I2" t="s">
         <v>29</v>
       </c>
-      <c r="J2">
-        <v>11414853</v>
+      <c r="J2" t="s">
+        <v>33</v>
       </c>
       <c r="L2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="M2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N2">
         <v>1</v>
       </c>
       <c r="O2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P2">
         <v>256</v>
@@ -651,22 +654,22 @@
         <v>20</v>
       </c>
       <c r="R2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="S2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="T2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="U2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="V2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="W2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="X2" t="s">
         <v>24</v>
@@ -695,16 +698,16 @@
         <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N3">
         <v>1</v>
       </c>
       <c r="O3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P3">
         <v>256</v>
@@ -713,22 +716,22 @@
         <v>20</v>
       </c>
       <c r="R3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="S3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="T3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="U3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="V3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="W3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="X3" t="s">
         <v>24</v>
@@ -753,20 +756,20 @@
       <c r="I4" t="s">
         <v>31</v>
       </c>
-      <c r="J4">
-        <v>11414853</v>
+      <c r="J4" t="s">
+        <v>33</v>
       </c>
       <c r="L4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="M4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N4">
         <v>1</v>
       </c>
       <c r="O4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P4">
         <v>256</v>
@@ -775,22 +778,22 @@
         <v>20</v>
       </c>
       <c r="R4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="S4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="T4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="U4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="V4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="W4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="X4" t="s">
         <v>24</v>
@@ -815,20 +818,20 @@
       <c r="I5" t="s">
         <v>32</v>
       </c>
-      <c r="J5">
-        <v>11414853</v>
+      <c r="J5" t="s">
+        <v>33</v>
       </c>
       <c r="L5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N5">
         <v>1</v>
       </c>
       <c r="O5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P5">
         <v>256</v>
@@ -837,22 +840,22 @@
         <v>20</v>
       </c>
       <c r="R5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="S5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="T5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="U5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="V5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="W5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="X5" t="s">
         <v>24</v>

</xml_diff>